<commit_message>
Check for locked Excel file and update tests.
</commit_message>
<xml_diff>
--- a/Test/singlecat keynotes.xlsx
+++ b/Test/singlecat keynotes.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Tim/Users/tim/Documents/code/dev/KN/Test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{A8059CBB-FFC3-A047-AD86-13BED73C27FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>General</t>
   </si>
   <si>
-    <t>REMEMBER TO SAVE after editing, then SAVE FILE AS Text (Tab delimited)(*.txt), then load/reload your keynotes on your project Revit file so Revit can see the changes. All keynote / text editing shall be on the Excel file only.</t>
+    <t>Mechanically generated keynote file. REMEMBER TO SAVE after editing, then SAVE FILE AS Text (Tab delimited)(*.txt), then load/reload your keynotes on your project Revit file so Revit can see the changes. All keynote / text editing shall be on the Excel file only.</t>
   </si>
   <si>
     <t>GENERAL</t>
@@ -83,40 +87,50 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="00FF0000"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <color rgb="00888888"/>
       <sz val="9"/>
+      <color rgb="FF888888"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <color rgb="0000FF00"/>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BBBBBB"/>
+        <fgColor rgb="FFBBBBBB"/>
       </patternFill>
     </fill>
   </fills>
@@ -130,25 +144,35 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -436,142 +460,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="2" min="2" width="100"/>
+    <col min="2" max="2" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
+      <c r="B2" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="6" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -580,6 +605,6 @@
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A18:C18"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>